<commit_message>
Replace spreadsheet info in README with 'How to Use' instructions in spreadsheets
</commit_message>
<xml_diff>
--- a/CT Dose Calculator.xlsx
+++ b/CT Dose Calculator.xlsx
@@ -20,7 +20,7 @@
     <definedName name="DLP">'CT Dose Calc'!$L$8</definedName>
     <definedName name="Dose">'CT Dose Calc'!$L$9</definedName>
   </definedNames>
-  <calcPr calcId="162913" iterateCount="1"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -821,13 +821,13 @@
       <xdr:col>14</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>19049</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>142874</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -836,8 +836,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8753475" y="19050"/>
-          <a:ext cx="3648075" cy="1800226"/>
+          <a:off x="8753475" y="19049"/>
+          <a:ext cx="3648075" cy="2600325"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -886,7 +886,9 @@
             <a:t> the appropriate values in the top portion of the </a:t>
           </a:r>
           <a:r>
-            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:rPr lang="en-US" sz="1000" b="0" baseline="0">
+              <a:latin typeface="Consolas" panose="020B0609020204030204" pitchFamily="49" charset="0"/>
+            </a:rPr>
             <a:t>Calculator</a:t>
           </a:r>
           <a:r>
@@ -900,8 +902,66 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-US" sz="1100" b="1"/>
-            <a:t>Technical Note:</a:t>
+            <a:t>Technical/Implementation Details:</a:t>
           </a:r>
+        </a:p>
+        <a:p>
+          <a:pPr marL="0" marR="0" lvl="0" indent="0" defTabSz="914400" eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1">
+            <a:lnSpc>
+              <a:spcPct val="100000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPts val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPts val="0"/>
+            </a:spcAft>
+            <a:buClrTx/>
+            <a:buSzTx/>
+            <a:buFontTx/>
+            <a:buNone/>
+            <a:tabLst/>
+            <a:defRPr/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Calculate and evaluate CT-only dose based on age and body site. Spreadsheet was originally created by King Turnbull</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> and was </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>heavily modified by Kaley White.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
         </a:p>
         <a:p>
           <a:r>
@@ -1228,7 +1288,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+      <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1650,6 +1710,7 @@
       <c r="H21" s="1"/>
     </row>
   </sheetData>
+  <sheetProtection sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="5">
     <mergeCell ref="K5:L5"/>
     <mergeCell ref="B2:L2"/>

</xml_diff>